<commit_message>
add uuid,fix delete function.
</commit_message>
<xml_diff>
--- a/ribao.xlsx
+++ b/ribao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="25320" windowHeight="12000" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="25320" windowHeight="11145" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="渗透测试" sheetId="1" state="visible" r:id="rId1"/>
@@ -1039,13 +1039,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1060,22 +1060,64 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>系统中文名</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>测试类别</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>测试进度</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>发现漏洞</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ZhangShan</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>e180c0d7-1485-4200-ab8e-dbb088a2bb97</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>系统名称1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>版本线</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>222222222</t>
         </is>
       </c>
     </row>
@@ -1091,10 +1133,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1112,20 +1154,25 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>系统名称</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>测试类别</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>审核通过漏洞</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>审核驳回漏洞</t>
         </is>
@@ -1143,13 +1190,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1164,61 +1211,22 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>系统中文名</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>测试进度</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>发现漏洞</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>陈浩</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-03-28</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>系统名称2</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>撒旦发射点发射点</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>陈浩</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-03-28</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>系统名称2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>士大夫随风倒</t>
         </is>
       </c>
     </row>
@@ -1233,13 +1241,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1254,44 +1262,22 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>审核平台</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>审核数量</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>审核结果</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>朱冠臻</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-03-28</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>IAST</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>豆腐干大概豆腐干</t>
         </is>
       </c>
     </row>
@@ -1306,15 +1292,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col width="12.375" customWidth="1" min="2" max="2"/>
+    <col width="12.375" customWidth="1" min="2" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1330,34 +1316,17 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>开发平台</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>开发内容</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>李杰</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-03-28</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>IAST</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>111111</t>
         </is>
       </c>
     </row>
@@ -1372,13 +1341,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1393,51 +1362,17 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>进度</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>编制内容</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>陈浩</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>90%</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>非如果他同意</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ZhangShan</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-03-29</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>搬砖100块。</t>
         </is>
       </c>
     </row>
@@ -1452,15 +1387,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col width="17.1833333333333" customWidth="1" min="2" max="2"/>
+    <col width="17.1833333333333" customWidth="1" min="2" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1476,6 +1411,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>UUID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>日报内容</t>
         </is>
       </c>
@@ -1488,12 +1428,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-03-29</t>
+          <t>2024-04-01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>打螺丝99枚。</t>
+          <t>b1f13017-a213-4a9f-9dbe-c40644dd8f7a</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2222222222</t>
         </is>
       </c>
     </row>

</xml_diff>